<commit_message>
Updated default aggregation table (2019, 2020) iea to exiobase
</commit_message>
<xml_diff>
--- a/inst/extdata/aggregation_table_iea_exiobase_2019.xlsx
+++ b/inst/extdata/aggregation_table_iea_exiobase_2019.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="aggregation_table" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="local_test" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="194">
   <si>
     <t xml:space="preserve">IEA_regions</t>
   </si>
@@ -31,37 +32,37 @@
     <t xml:space="preserve">World</t>
   </si>
   <si>
-    <t xml:space="preserve">OECD Americas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OECD Asia Oceania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OECD Europe</t>
+    <t xml:space="preserve">OECD Americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OECD Asia Oceania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OECD Europe</t>
   </si>
   <si>
     <t xml:space="preserve">Africa</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-OECD Americas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle East</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-OECD Europe and Eurasia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-OECD Asia (excluding China)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China (P.R. of China and Hong Kong, China)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World marine bunkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World aviation bunkers</t>
+    <t xml:space="preserve">Non-OECD Americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-OECD Europe and Eurasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-OECD Asia (excluding China)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China (P.R. of China and Hong Kong, China)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World marine bunkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World aviation bunkers</t>
   </si>
   <si>
     <t xml:space="preserve">Albania</t>
@@ -118,10 +119,10 @@
     <t xml:space="preserve">Benin</t>
   </si>
   <si>
-    <t xml:space="preserve">Plurinational State of Bolivia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bosnia and Herzegovina</t>
+    <t xml:space="preserve">Plurinational State of Bolivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosnia and Herzegovina</t>
   </si>
   <si>
     <t xml:space="preserve">Botswana</t>
@@ -130,7 +131,7 @@
     <t xml:space="preserve">Brazil</t>
   </si>
   <si>
-    <t xml:space="preserve">Brunei Darussalam</t>
+    <t xml:space="preserve">Brunei Darussalam</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria</t>
@@ -148,7 +149,7 @@
     <t xml:space="preserve">Chile</t>
   </si>
   <si>
-    <t xml:space="preserve">People's Republic of China</t>
+    <t xml:space="preserve">People's Republic of China</t>
   </si>
   <si>
     <t xml:space="preserve">China</t>
@@ -157,10 +158,10 @@
     <t xml:space="preserve">Colombia</t>
   </si>
   <si>
-    <t xml:space="preserve">Republic of the Congo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costa Rica</t>
+    <t xml:space="preserve">Republic of the Congo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costa Rica</t>
   </si>
   <si>
     <t xml:space="preserve">Côte d'Ivoire</t>
@@ -175,25 +176,25 @@
     <t xml:space="preserve">Curaçao/Netherlands Antilles</t>
   </si>
   <si>
+    <t xml:space="preserve">TESTING</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cyprus</t>
   </si>
   <si>
-    <t xml:space="preserve">Czech Republic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Czech Republic</t>
   </si>
   <si>
-    <t xml:space="preserve">Democratic People's Republic of Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Democratic Republic of the Congo</t>
+    <t xml:space="preserve">Democratic People's Republic of Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic Republic of the Congo</t>
   </si>
   <si>
     <t xml:space="preserve">Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">Dominican Republic</t>
+    <t xml:space="preserve">Dominican Republic</t>
   </si>
   <si>
     <t xml:space="preserve">Ecuador</t>
@@ -202,7 +203,7 @@
     <t xml:space="preserve">Egypt</t>
   </si>
   <si>
-    <t xml:space="preserve">El Salvador</t>
+    <t xml:space="preserve">El Salvador</t>
   </si>
   <si>
     <t xml:space="preserve">Eritrea</t>
@@ -247,7 +248,7 @@
     <t xml:space="preserve">Honduras</t>
   </si>
   <si>
-    <t xml:space="preserve">Hong Kong (China)</t>
+    <t xml:space="preserve">Hong Kong (China)</t>
   </si>
   <si>
     <t xml:space="preserve">Hungary</t>
@@ -262,7 +263,7 @@
     <t xml:space="preserve">Indonesia</t>
   </si>
   <si>
-    <t xml:space="preserve">Islamic Republic of Iran</t>
+    <t xml:space="preserve">Islamic Republic of Iran</t>
   </si>
   <si>
     <t xml:space="preserve">Iraq</t>
@@ -334,7 +335,7 @@
     <t xml:space="preserve">Mexico</t>
   </si>
   <si>
-    <t xml:space="preserve">Republic of Moldova</t>
+    <t xml:space="preserve">Republic of Moldova</t>
   </si>
   <si>
     <t xml:space="preserve">Mongolia</t>
@@ -361,7 +362,7 @@
     <t xml:space="preserve">Netherlands</t>
   </si>
   <si>
-    <t xml:space="preserve">New Zealand</t>
+    <t xml:space="preserve">New Zealand</t>
   </si>
   <si>
     <t xml:space="preserve">Nicaragua</t>
@@ -373,7 +374,7 @@
     <t xml:space="preserve">Nigeria</t>
   </si>
   <si>
-    <t xml:space="preserve">Republic of North Macedonia</t>
+    <t xml:space="preserve">Republic of North Macedonia</t>
   </si>
   <si>
     <t xml:space="preserve">Norway</t>
@@ -409,13 +410,10 @@
     <t xml:space="preserve">Romania</t>
   </si>
   <si>
-    <t xml:space="preserve">Russian Federation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Russian Federation</t>
   </si>
   <si>
-    <t xml:space="preserve">Saudi Arabia</t>
+    <t xml:space="preserve">Saudi Arabia</t>
   </si>
   <si>
     <t xml:space="preserve">Senegal</t>
@@ -427,9 +425,6 @@
     <t xml:space="preserve">Singapore</t>
   </si>
   <si>
-    <t xml:space="preserve">Slovak Republic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Slovak Republic</t>
   </si>
   <si>
@@ -439,13 +434,13 @@
     <t xml:space="preserve">South Africa</t>
   </si>
   <si>
-    <t xml:space="preserve">South Sudan</t>
+    <t xml:space="preserve">South Sudan</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Sri Lanka</t>
+    <t xml:space="preserve">Sri Lanka</t>
   </si>
   <si>
     <t xml:space="preserve">Sudan</t>
@@ -460,10 +455,10 @@
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chinese Taipei</t>
+    <t xml:space="preserve">Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese Taipei</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan</t>
@@ -472,7 +467,7 @@
     <t xml:space="preserve">Tajikistan</t>
   </si>
   <si>
-    <t xml:space="preserve">United Republic of Tanzania</t>
+    <t xml:space="preserve">United Republic of Tanzania</t>
   </si>
   <si>
     <t xml:space="preserve">Thailand</t>
@@ -481,7 +476,7 @@
     <t xml:space="preserve">Togo</t>
   </si>
   <si>
-    <t xml:space="preserve">Trinidad and Tobago</t>
+    <t xml:space="preserve">Trinidad and Tobago</t>
   </si>
   <si>
     <t xml:space="preserve">Tunisia</t>
@@ -496,18 +491,12 @@
     <t xml:space="preserve">Ukraine</t>
   </si>
   <si>
-    <t xml:space="preserve">United Arab Emirates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
+    <t xml:space="preserve">United Arab Emirates</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">United States</t>
-  </si>
-  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -517,10 +506,10 @@
     <t xml:space="preserve">Uzbekistan</t>
   </si>
   <si>
-    <t xml:space="preserve">Bolivarian Republic of Venezuela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viet Nam</t>
+    <t xml:space="preserve">Bolivarian Republic of Venezuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viet Nam</t>
   </si>
   <si>
     <t xml:space="preserve">Yemen</t>
@@ -532,88 +521,88 @@
     <t xml:space="preserve">Zimbabwe</t>
   </si>
   <si>
-    <t xml:space="preserve">Former Soviet Union (If no detail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Former Yugoslavia (If no detail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other non-OECD Americas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other non-OECD Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Equatorial Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Greenland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Lao People's Democratic Republic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Mali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Palestinian Authority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Uganda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Africa (UN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Americas (UN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Asia (UN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Europe (UN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Oceania (UN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: OECD Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Non-OECD Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: IEA Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: IEA and Accession/Association countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: European Union-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: FSU 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: Former Yugoslavia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: OPEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: ASEAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: G7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: G8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memo: G20</t>
+    <t xml:space="preserve">Former Soviet Union (If no detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Former Yugoslavia (If no detail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other non-OECD Americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other non-OECD Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Equatorial Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Greenland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Mali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Palestinian Authority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Uganda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Africa (UN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Americas (UN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Asia (UN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Europe (UN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Oceania (UN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: OECD Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Non-OECD Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: IEA Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: IEA and Accession/Association countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: European Union-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: FSU 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: Former Yugoslavia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: OPEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: ASEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: G7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: G8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo: G20</t>
   </si>
 </sst>
 </file>
@@ -729,8 +718,8 @@
   </sheetPr>
   <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1064,19 +1053,21 @@
       <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>53</v>
@@ -1673,12 +1664,12 @@
         <v>129</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>27</v>
@@ -1686,7 +1677,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>17</v>
@@ -1694,7 +1685,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>15</v>
@@ -1702,7 +1693,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>22</v>
@@ -1710,45 +1701,45 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>22</v>
@@ -1756,7 +1747,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>17</v>
@@ -1764,7 +1755,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>20</v>
@@ -1772,23 +1763,23 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>27</v>
@@ -1796,15 +1787,15 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>22</v>
@@ -1812,7 +1803,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>17</v>
@@ -1820,7 +1811,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>22</v>
@@ -1828,7 +1819,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>17</v>
@@ -1836,7 +1827,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>20</v>
@@ -1844,7 +1835,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>17</v>
@@ -1852,15 +1843,15 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>22</v>
@@ -1868,7 +1859,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>15</v>
@@ -1876,7 +1867,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>27</v>
@@ -1884,23 +1875,23 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>20</v>
@@ -1908,7 +1899,7 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>22</v>
@@ -1916,7 +1907,7 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>20</v>
@@ -1924,7 +1915,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>22</v>
@@ -1932,7 +1923,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>27</v>
@@ -1940,7 +1931,7 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>17</v>
@@ -1948,7 +1939,7 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>17</v>
@@ -1956,19 +1947,19 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B157" s="2"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B158" s="2"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>17</v>
@@ -1976,7 +1967,7 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>20</v>
@@ -1984,7 +1975,7 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>22</v>
@@ -1992,13 +1983,13 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B162" s="2"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>20</v>
@@ -2006,127 +1997,127 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B164" s="2"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B165" s="2"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B166" s="2"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B167" s="2"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B168" s="2"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B169" s="2"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B170" s="2"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B171" s="2"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B172" s="2"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B173" s="2"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B174" s="2"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B175" s="2"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B176" s="2"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B177" s="2"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B178" s="2"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B179" s="2"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B180" s="2"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B181" s="2"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B182" s="2"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B183" s="2"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B184" s="2"/>
     </row>
@@ -2153,4 +2144,1505 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B184"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B179" activeCellId="0" sqref="B179"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>